<commit_message>
Refactor : Refactoring Cli programs
Added 4 modules:
	Analyze, Grade, Register, Util
</commit_message>
<xml_diff>
--- a/data/h모의고사/제출답안.xlsx
+++ b/data/h모의고사/제출답안.xlsx
@@ -1,27 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\송종빈\PycharmProjects\sonexam\data\h모의고사\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isanghun/grade_analysis/data/h모의고사/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175B9102-E7C6-4B59-867D-CA2746EA0B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BE662C-4C6F-E847-8A51-31A665A4863D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3760" yWindow="1380" windowWidth="17280" windowHeight="8960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="제출답안" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>학생 이름</t>
   </si>
@@ -49,6 +60,18 @@
   </si>
   <si>
     <t>54321543215432154321</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -56,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,9 +426,9 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="3" max="3" width="26.8984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -419,12 +442,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,7 +458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -446,7 +469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -457,8 +480,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="C4" s="1"/>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>